<commit_message>
Add support for files and adding the parent column relationships
</commit_message>
<xml_diff>
--- a/storage/test_data/etl/d1_headers.xlsx
+++ b/storage/test_data/etl/d1_headers.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="11">
   <si>
     <t xml:space="preserve">NAME</t>
   </si>
@@ -47,6 +47,12 @@
   </si>
   <si>
     <t xml:space="preserve">S:bead width (mm)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">file:text:p1/d1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">file:p1</t>
   </si>
 </sst>
 </file>
@@ -153,7 +159,7 @@
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="bottomLeft" activeCell="I10" activeCellId="0" sqref="I10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -201,6 +207,12 @@
       </c>
       <c r="J1" s="1" t="s">
         <v>8</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>10</v>
       </c>
       <c r="ALT1" s="0"/>
       <c r="ALU1" s="0"/>
@@ -233,6 +245,10 @@
     <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="K1" r:id="rId1" display="file:text:p1/d1"/>
+    <hyperlink ref="L1" r:id="rId2" display="file:p1"/>
+  </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
   <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>

</xml_diff>